<commit_message>
adding some notes to recently recorded mice.
</commit_message>
<xml_diff>
--- a/CH_032414_A.xlsx
+++ b/CH_032414_A.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charlie\Documents\SourceTree_local\docubase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glickfeld_lab\Documents\docubase\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1185" yWindow="135" windowWidth="25605" windowHeight="16065" tabRatio="624" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="1185" yWindow="135" windowWidth="25605" windowHeight="16065" tabRatio="624"/>
   </bookViews>
   <sheets>
     <sheet name="General Info" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="102">
   <si>
     <t>Mouse ID</t>
   </si>
@@ -144,10 +144,196 @@
     <t>EMX-Cre +/-</t>
   </si>
   <si>
-    <t>Injected AAV1.ChR2 into V1.</t>
-  </si>
-  <si>
-    <t>None, but I should punch one of the ears to distinguish from EB mice</t>
+    <t>both ears wedged.</t>
+  </si>
+  <si>
+    <t>2014_04_06_0000</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>Unknown cell type in L2/3. Round cell body, and I think non-adapting, but no sharp repolarization…</t>
+  </si>
+  <si>
+    <t>2014_04_06_0001</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>Strong tdTomato signal in the thalamus, but only weak signal in the cortex.</t>
+  </si>
+  <si>
+    <t>Blue light steps at soma (0 0). FS open. Good access. No responses at any voltage to the LED. Moving on…</t>
+  </si>
+  <si>
+    <t>2014_04_06_0002</t>
+  </si>
+  <si>
+    <t>Blue light steps from a rather un-healthy looking PY cell in L5. Very weak responses even at the highest light levels.</t>
+  </si>
+  <si>
+    <t>2014_04_06_0003</t>
+  </si>
+  <si>
+    <t>2014_04_06_0004</t>
+  </si>
+  <si>
+    <t>chelator pulses</t>
+  </si>
+  <si>
+    <t>chelator pulses repeats</t>
+  </si>
+  <si>
+    <t>2014_04_06_0005</t>
+  </si>
+  <si>
+    <t>chelator pulses 1 minute after washing on EGTA. I added 20ul of EGTA-AM (100mM) to 100 ml of normal ACSF.</t>
+  </si>
+  <si>
+    <t>2014_04_06_0006</t>
+  </si>
+  <si>
+    <t>chlelator pulses repeats. All files with EGTA targted the soma with the FS open.</t>
+  </si>
+  <si>
+    <t>out</t>
+  </si>
+  <si>
+    <t>Strange burst-tonic behavior to current injections in EGTA…</t>
+  </si>
+  <si>
+    <t>Vout = 9 mV. Picture on crash.</t>
+  </si>
+  <si>
+    <t>2014_04_06_0007</t>
+  </si>
+  <si>
+    <t>2014_04_06_0008</t>
+  </si>
+  <si>
+    <t>2014_04_06_0009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DC steps from a L2/3 PY cell. </t>
+  </si>
+  <si>
+    <t>2014_04_06_0010</t>
+  </si>
+  <si>
+    <t>Blue light steps targeted to the soma (0 0). Strangely poor access for how big the pipette is… Weak responses only at the highest light powers</t>
+  </si>
+  <si>
+    <t>2014_04_06_0011</t>
+  </si>
+  <si>
+    <t>2014_04_06_0012</t>
+  </si>
+  <si>
+    <t>2014_04_06_0013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blue light trains targeted to the soma with the FS iris open. 20Hz trains. LED voltage was 10 V. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blue light trains targeted to the soma with the FS iris open. 5 Hz trains. LED voltage was 10 V. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blue light trains targeted to the soma with the FS iris open. 40 Hz trains. LED voltage was 10 V. </t>
+  </si>
+  <si>
+    <t>2014_04_06_0014</t>
+  </si>
+  <si>
+    <t>LED 470 nm steps targeted to (-181 247). No response.</t>
+  </si>
+  <si>
+    <t>Picture uses a 1.5 sec exposure. So the expression is actually not that great. Vout = 6 mV.</t>
+  </si>
+  <si>
+    <t>Hippocampus is starting to form dorsally. Weak signal in the visual thalamus. Pretty weak cortical expression. Callosum is not yet fused.</t>
+  </si>
+  <si>
+    <t>2014_04_06_0016</t>
+  </si>
+  <si>
+    <t>gap free</t>
+  </si>
+  <si>
+    <t>2014_04_06_0017</t>
+  </si>
+  <si>
+    <t>gap free. Vm isn't sttable at all…</t>
+  </si>
+  <si>
+    <t>2014_04_06_0018</t>
+  </si>
+  <si>
+    <t>2014_04_06_0019</t>
+  </si>
+  <si>
+    <t>2014_04_06_0020</t>
+  </si>
+  <si>
+    <t>2014_04_06_0021</t>
+  </si>
+  <si>
+    <t>junk</t>
+  </si>
+  <si>
+    <t>LED 470 nm trains at 20 Hz. Might need a slightly higher LED voltage. At the soma. FS open.</t>
+  </si>
+  <si>
+    <t>2014_04_06_0022</t>
+  </si>
+  <si>
+    <t>2014_04_06_0023</t>
+  </si>
+  <si>
+    <t>2014_04_06_0024</t>
+  </si>
+  <si>
+    <t>LED 470 nm trains at 20 Hz. LED set to 2.5 volts.. At the soma. FS open.</t>
+  </si>
+  <si>
+    <t>LED 470 nm trains at 5 Hz. LED set to 2.5 volts.. At the soma. FS open. Access got a little worse.</t>
+  </si>
+  <si>
+    <t>LED 470 nm trains at 40 Hz. LED set to 2.5 volts.. At the soma. FS open. Access got a little worse.</t>
+  </si>
+  <si>
+    <t>2014_04_06_0025</t>
+  </si>
+  <si>
+    <t>LED 470 nm steps at (-352 59). Very weak response at all light powers. Access is quite bad now.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blue light steps at the soma. This cell isn't exactly at (0 0) but I forgot to write it down.... FS open. Good responses when the LED is set to 2.5 volts. </t>
+  </si>
+  <si>
+    <t>No picture on crash. I accidently retracted the electrode before I could take a picture. The upshot is that this neuron is superficially located but I had trouble evoking PSCs with the FS iris closed at all of the locations I tried to stimulate (much data not saved b/c there was no response). Weak responses in superficial cortex.</t>
+  </si>
+  <si>
+    <t>DC steps from a L2/3 PY cell. This is proably area LM or area P. Since it doesn't look like CA3 is in view, it's likely that this HOA is P.</t>
+  </si>
+  <si>
+    <t>No CA3. One area lateral to the injection site. The injection site has good signal in deep layers, but only marginal signal in superficial layers.</t>
+  </si>
+  <si>
+    <t>K-Gluconate ('busted')</t>
+  </si>
+  <si>
+    <t>Normal. One cell used EGTA-AM</t>
+  </si>
+  <si>
+    <t>34 degrees, checked by hand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hard to record today. Fairly weak ChR2 expression. No cortex damage, but I think the injection was too deep, and that I didn't inject enough. </t>
+  </si>
+  <si>
+    <t>Injected AAV1.ChR2 into V1. Fairly weak expression despite no cortical damage. Perhaps the injection was too deep, or I didn't inject enough virus. Seems like 100 nl should be the low limit for virus injections of AAV2/1.CAG.flexed.ChR2.tdTomato. And 350 um from pia seems reasonable.</t>
   </si>
 </sst>
 </file>
@@ -686,7 +872,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -786,6 +972,9 @@
     </xf>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1271,8 +1460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B6"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="38.1" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -1319,7 +1508,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="147.94999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1327,7 +1516,7 @@
         <v>21</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>38</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="38.1" hidden="1" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
@@ -1356,13 +1545,13 @@
   <dimension ref="A1:H101"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C4" sqref="C4:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13" style="1" customWidth="1"/>
     <col min="3" max="3" width="6.875" style="1" customWidth="1"/>
     <col min="4" max="4" width="7.125" style="1" customWidth="1"/>
     <col min="5" max="5" width="7.125" style="21" customWidth="1"/>
@@ -1373,66 +1562,78 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="39" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="55" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
       <c r="G1" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="22"/>
+      <c r="H1" s="22">
+        <v>297</v>
+      </c>
     </row>
     <row r="2" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
       <c r="G2" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="24"/>
+      <c r="H2" s="24">
+        <v>309</v>
+      </c>
     </row>
     <row r="3" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="43"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="42" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="44"/>
     </row>
     <row r="4" spans="1:8" ht="102" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="53"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="47"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="45" t="s">
+        <v>100</v>
+      </c>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="48"/>
     </row>
     <row r="5" spans="1:8" ht="26.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="40"/>
-      <c r="B5" s="40"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
+      <c r="A5" s="41"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
     </row>
     <row r="6" spans="1:8" ht="39" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
@@ -1450,41 +1651,69 @@
       <c r="E6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="37" t="s">
+      <c r="F6" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="38"/>
-      <c r="H6" s="39"/>
-    </row>
-    <row r="7" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G6" s="39"/>
+      <c r="H6" s="40"/>
+    </row>
+    <row r="7" spans="1:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
-      <c r="D7" s="5"/>
+      <c r="D7" s="5">
+        <v>7</v>
+      </c>
       <c r="E7" s="23"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="36"/>
+      <c r="F7" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="36"/>
+      <c r="H7" s="37"/>
     </row>
     <row r="8" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="36"/>
-    </row>
-    <row r="9" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="36"/>
+      <c r="A8" s="3">
+        <v>1</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="5">
+        <v>7</v>
+      </c>
+      <c r="E8" s="23">
+        <v>-65</v>
+      </c>
+      <c r="F8" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="36"/>
+      <c r="H8" s="37"/>
+    </row>
+    <row r="9" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>1</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="5">
+        <v>7</v>
+      </c>
+      <c r="E9" s="23">
+        <v>-85</v>
+      </c>
+      <c r="F9" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" s="36"/>
+      <c r="H9" s="37"/>
     </row>
     <row r="10" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
@@ -1492,89 +1721,179 @@
       <c r="C10" s="4"/>
       <c r="D10" s="5"/>
       <c r="E10" s="23"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="36"/>
-    </row>
-    <row r="11" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="36"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="37"/>
+    </row>
+    <row r="11" spans="1:8" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>2</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="5">
+        <v>7</v>
+      </c>
+      <c r="E11" s="23">
+        <v>-85</v>
+      </c>
+      <c r="F11" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" s="36"/>
+      <c r="H11" s="37"/>
     </row>
     <row r="12" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="36"/>
+      <c r="A12" s="3">
+        <v>2</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="34">
+        <v>7</v>
+      </c>
+      <c r="E12" s="23">
+        <v>-85</v>
+      </c>
+      <c r="F12" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="G12" s="36"/>
+      <c r="H12" s="37"/>
     </row>
     <row r="13" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="36"/>
-    </row>
-    <row r="14" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="36"/>
+      <c r="A13" s="3">
+        <v>2</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="34">
+        <v>7</v>
+      </c>
+      <c r="E13" s="23">
+        <v>-85</v>
+      </c>
+      <c r="F13" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" s="36"/>
+      <c r="H13" s="37"/>
+    </row>
+    <row r="14" spans="1:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>2</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="34">
+        <v>7</v>
+      </c>
+      <c r="E14" s="34">
+        <v>-85</v>
+      </c>
+      <c r="F14" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" s="36"/>
+      <c r="H14" s="37"/>
     </row>
     <row r="15" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="36"/>
+      <c r="A15" s="3">
+        <v>2</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="34">
+        <v>7</v>
+      </c>
+      <c r="E15" s="34">
+        <v>-85</v>
+      </c>
+      <c r="F15" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="G15" s="36"/>
+      <c r="H15" s="37"/>
     </row>
     <row r="16" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="36"/>
+      <c r="A16" s="3">
+        <v>2</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="34">
+        <v>7</v>
+      </c>
+      <c r="E16" s="34">
+        <v>-85</v>
+      </c>
+      <c r="F16" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="G16" s="36"/>
+      <c r="H16" s="37"/>
     </row>
     <row r="17" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="35"/>
-      <c r="H17" s="36"/>
+      <c r="A17" s="3">
+        <v>2</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="34">
+        <v>7</v>
+      </c>
+      <c r="E17" s="34"/>
+      <c r="F17" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="G17" s="36"/>
+      <c r="H17" s="37"/>
     </row>
     <row r="18" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
+      <c r="A18" s="3">
+        <v>2</v>
+      </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="36"/>
+      <c r="D18" s="34">
+        <v>7</v>
+      </c>
+      <c r="E18" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="F18" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="G18" s="36"/>
+      <c r="H18" s="37"/>
     </row>
     <row r="19" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
@@ -1582,89 +1901,173 @@
       <c r="C19" s="4"/>
       <c r="D19" s="5"/>
       <c r="E19" s="23"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="36"/>
-    </row>
-    <row r="20" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F19" s="35"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="37"/>
+    </row>
+    <row r="20" spans="1:8" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
-      <c r="D20" s="5"/>
+      <c r="D20" s="5">
+        <v>5</v>
+      </c>
       <c r="E20" s="23"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="35"/>
-      <c r="H20" s="36"/>
+      <c r="F20" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="G20" s="36"/>
+      <c r="H20" s="37"/>
     </row>
     <row r="21" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="34"/>
-      <c r="G21" s="35"/>
-      <c r="H21" s="36"/>
-    </row>
-    <row r="22" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="35"/>
-      <c r="H22" s="36"/>
-    </row>
-    <row r="23" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="35"/>
-      <c r="H23" s="36"/>
+      <c r="A21" s="3">
+        <v>3</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="5">
+        <v>5</v>
+      </c>
+      <c r="E21" s="23">
+        <v>-82</v>
+      </c>
+      <c r="F21" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="G21" s="36"/>
+      <c r="H21" s="37"/>
+    </row>
+    <row r="22" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>3</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="34">
+        <v>5</v>
+      </c>
+      <c r="E22" s="23">
+        <v>-85</v>
+      </c>
+      <c r="F22" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="G22" s="36"/>
+      <c r="H22" s="37"/>
+    </row>
+    <row r="23" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>3</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23" s="34">
+        <v>5</v>
+      </c>
+      <c r="E23" s="34">
+        <v>-85</v>
+      </c>
+      <c r="F23" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="G23" s="36"/>
+      <c r="H23" s="37"/>
     </row>
     <row r="24" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="35"/>
-      <c r="H24" s="36"/>
+      <c r="A24" s="3">
+        <v>3</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" s="34">
+        <v>5</v>
+      </c>
+      <c r="E24" s="34">
+        <v>-85</v>
+      </c>
+      <c r="F24" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="G24" s="36"/>
+      <c r="H24" s="37"/>
     </row>
     <row r="25" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="34"/>
-      <c r="G25" s="35"/>
-      <c r="H25" s="36"/>
+      <c r="A25" s="3">
+        <v>3</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" s="34">
+        <v>5</v>
+      </c>
+      <c r="E25" s="34">
+        <v>-85</v>
+      </c>
+      <c r="F25" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="G25" s="36"/>
+      <c r="H25" s="37"/>
     </row>
     <row r="26" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="35"/>
-      <c r="H26" s="36"/>
+      <c r="A26" s="3">
+        <v>3</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" s="34">
+        <v>5</v>
+      </c>
+      <c r="E26" s="34">
+        <v>-85</v>
+      </c>
+      <c r="F26" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="G26" s="36"/>
+      <c r="H26" s="37"/>
     </row>
     <row r="27" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
+      <c r="A27" s="3">
+        <v>3</v>
+      </c>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="35"/>
-      <c r="H27" s="36"/>
+      <c r="D27" s="34">
+        <v>5</v>
+      </c>
+      <c r="E27" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="F27" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="G27" s="36"/>
+      <c r="H27" s="37"/>
     </row>
     <row r="28" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
@@ -1672,39 +2075,63 @@
       <c r="C28" s="4"/>
       <c r="D28" s="5"/>
       <c r="E28" s="23"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="35"/>
-      <c r="H28" s="36"/>
-    </row>
-    <row r="29" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F28" s="35"/>
+      <c r="G28" s="36"/>
+      <c r="H28" s="37"/>
+    </row>
+    <row r="29" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
-      <c r="D29" s="5"/>
+      <c r="D29" s="5">
+        <v>3</v>
+      </c>
       <c r="E29" s="23"/>
-      <c r="F29" s="34"/>
-      <c r="G29" s="35"/>
-      <c r="H29" s="36"/>
+      <c r="F29" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="G29" s="36"/>
+      <c r="H29" s="37"/>
     </row>
     <row r="30" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="5"/>
+      <c r="A30" s="3">
+        <v>4</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30" s="5">
+        <v>3</v>
+      </c>
       <c r="E30" s="23"/>
-      <c r="F30" s="34"/>
-      <c r="G30" s="35"/>
-      <c r="H30" s="36"/>
+      <c r="F30" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="G30" s="36"/>
+      <c r="H30" s="37"/>
     </row>
     <row r="31" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="5"/>
+      <c r="A31" s="3">
+        <v>4</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D31" s="5">
+        <v>3</v>
+      </c>
       <c r="E31" s="23"/>
-      <c r="F31" s="34"/>
-      <c r="G31" s="35"/>
-      <c r="H31" s="36"/>
+      <c r="F31" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="G31" s="36"/>
+      <c r="H31" s="37"/>
     </row>
     <row r="32" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
@@ -1712,99 +2139,203 @@
       <c r="C32" s="4"/>
       <c r="D32" s="5"/>
       <c r="E32" s="23"/>
-      <c r="F32" s="34"/>
-      <c r="G32" s="35"/>
-      <c r="H32" s="36"/>
-    </row>
-    <row r="33" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="3"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="23"/>
-      <c r="F33" s="34"/>
-      <c r="G33" s="35"/>
-      <c r="H33" s="36"/>
-    </row>
-    <row r="34" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="23"/>
-      <c r="F34" s="34"/>
-      <c r="G34" s="35"/>
-      <c r="H34" s="36"/>
+      <c r="F32" s="35"/>
+      <c r="G32" s="36"/>
+      <c r="H32" s="37"/>
+    </row>
+    <row r="33" spans="1:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
+        <v>5</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D33" s="5">
+        <v>3</v>
+      </c>
+      <c r="E33" s="23">
+        <v>-83</v>
+      </c>
+      <c r="F33" s="35" t="s">
+        <v>95</v>
+      </c>
+      <c r="G33" s="36"/>
+      <c r="H33" s="37"/>
+    </row>
+    <row r="34" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="3">
+        <v>5</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D34" s="34">
+        <v>3</v>
+      </c>
+      <c r="E34" s="23">
+        <v>-85</v>
+      </c>
+      <c r="F34" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="G34" s="36"/>
+      <c r="H34" s="37"/>
     </row>
     <row r="35" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="3"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="34"/>
-      <c r="G35" s="35"/>
-      <c r="H35" s="36"/>
+      <c r="A35" s="3">
+        <v>5</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D35" s="34">
+        <v>3</v>
+      </c>
+      <c r="E35" s="34">
+        <v>-85</v>
+      </c>
+      <c r="F35" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="G35" s="36"/>
+      <c r="H35" s="37"/>
     </row>
     <row r="36" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="3"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="23"/>
-      <c r="F36" s="34"/>
-      <c r="G36" s="35"/>
-      <c r="H36" s="36"/>
+      <c r="A36" s="3">
+        <v>5</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D36" s="34">
+        <v>3</v>
+      </c>
+      <c r="E36" s="34">
+        <v>-85</v>
+      </c>
+      <c r="F36" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="G36" s="36"/>
+      <c r="H36" s="37"/>
     </row>
     <row r="37" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="3"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="23"/>
-      <c r="F37" s="34"/>
-      <c r="G37" s="35"/>
-      <c r="H37" s="36"/>
-    </row>
-    <row r="38" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="3"/>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="23"/>
-      <c r="F38" s="34"/>
-      <c r="G38" s="35"/>
-      <c r="H38" s="36"/>
+      <c r="A37" s="3">
+        <v>5</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D37" s="34">
+        <v>3</v>
+      </c>
+      <c r="E37" s="34">
+        <v>-85</v>
+      </c>
+      <c r="F37" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="G37" s="36"/>
+      <c r="H37" s="37"/>
+    </row>
+    <row r="38" spans="1:8" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="3">
+        <v>5</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D38" s="34">
+        <v>3</v>
+      </c>
+      <c r="E38" s="34">
+        <v>-85</v>
+      </c>
+      <c r="F38" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="G38" s="36"/>
+      <c r="H38" s="37"/>
     </row>
     <row r="39" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="3"/>
-      <c r="B39" s="4"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="23"/>
-      <c r="F39" s="34"/>
-      <c r="G39" s="35"/>
-      <c r="H39" s="36"/>
-    </row>
-    <row r="40" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
-      <c r="B40" s="4"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="23"/>
-      <c r="F40" s="34"/>
-      <c r="G40" s="35"/>
-      <c r="H40" s="36"/>
-    </row>
-    <row r="41" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="3"/>
+      <c r="A39" s="3">
+        <v>5</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D39" s="34">
+        <v>3</v>
+      </c>
+      <c r="E39" s="34">
+        <v>-85</v>
+      </c>
+      <c r="F39" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="G39" s="36"/>
+      <c r="H39" s="37"/>
+    </row>
+    <row r="40" spans="1:8" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="3">
+        <v>5</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D40" s="34">
+        <v>3</v>
+      </c>
+      <c r="E40" s="34">
+        <v>-85</v>
+      </c>
+      <c r="F40" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="G40" s="36"/>
+      <c r="H40" s="37"/>
+    </row>
+    <row r="41" spans="1:8" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="3">
+        <v>5</v>
+      </c>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="23"/>
-      <c r="F41" s="34"/>
-      <c r="G41" s="35"/>
-      <c r="H41" s="36"/>
+      <c r="D41" s="34">
+        <v>3</v>
+      </c>
+      <c r="E41" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="F41" s="35" t="s">
+        <v>94</v>
+      </c>
+      <c r="G41" s="36"/>
+      <c r="H41" s="37"/>
     </row>
     <row r="42" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
@@ -1812,9 +2343,9 @@
       <c r="C42" s="4"/>
       <c r="D42" s="5"/>
       <c r="E42" s="23"/>
-      <c r="F42" s="34"/>
-      <c r="G42" s="35"/>
-      <c r="H42" s="36"/>
+      <c r="F42" s="35"/>
+      <c r="G42" s="36"/>
+      <c r="H42" s="37"/>
     </row>
     <row r="43" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
@@ -1822,9 +2353,9 @@
       <c r="C43" s="4"/>
       <c r="D43" s="5"/>
       <c r="E43" s="23"/>
-      <c r="F43" s="34"/>
-      <c r="G43" s="35"/>
-      <c r="H43" s="36"/>
+      <c r="F43" s="35"/>
+      <c r="G43" s="36"/>
+      <c r="H43" s="37"/>
     </row>
     <row r="44" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
@@ -1832,9 +2363,9 @@
       <c r="C44" s="4"/>
       <c r="D44" s="5"/>
       <c r="E44" s="23"/>
-      <c r="F44" s="34"/>
-      <c r="G44" s="35"/>
-      <c r="H44" s="36"/>
+      <c r="F44" s="35"/>
+      <c r="G44" s="36"/>
+      <c r="H44" s="37"/>
     </row>
     <row r="45" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
@@ -1842,9 +2373,9 @@
       <c r="C45" s="4"/>
       <c r="D45" s="5"/>
       <c r="E45" s="23"/>
-      <c r="F45" s="34"/>
-      <c r="G45" s="35"/>
-      <c r="H45" s="36"/>
+      <c r="F45" s="35"/>
+      <c r="G45" s="36"/>
+      <c r="H45" s="37"/>
     </row>
     <row r="46" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
@@ -1852,9 +2383,9 @@
       <c r="C46" s="4"/>
       <c r="D46" s="5"/>
       <c r="E46" s="23"/>
-      <c r="F46" s="34"/>
-      <c r="G46" s="35"/>
-      <c r="H46" s="36"/>
+      <c r="F46" s="35"/>
+      <c r="G46" s="36"/>
+      <c r="H46" s="37"/>
     </row>
     <row r="47" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
@@ -1862,9 +2393,9 @@
       <c r="C47" s="4"/>
       <c r="D47" s="5"/>
       <c r="E47" s="23"/>
-      <c r="F47" s="34"/>
-      <c r="G47" s="35"/>
-      <c r="H47" s="36"/>
+      <c r="F47" s="35"/>
+      <c r="G47" s="36"/>
+      <c r="H47" s="37"/>
     </row>
     <row r="48" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
@@ -1872,9 +2403,9 @@
       <c r="C48" s="4"/>
       <c r="D48" s="5"/>
       <c r="E48" s="23"/>
-      <c r="F48" s="34"/>
-      <c r="G48" s="35"/>
-      <c r="H48" s="36"/>
+      <c r="F48" s="35"/>
+      <c r="G48" s="36"/>
+      <c r="H48" s="37"/>
     </row>
     <row r="49" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
@@ -1882,9 +2413,9 @@
       <c r="C49" s="4"/>
       <c r="D49" s="5"/>
       <c r="E49" s="23"/>
-      <c r="F49" s="34"/>
-      <c r="G49" s="35"/>
-      <c r="H49" s="36"/>
+      <c r="F49" s="35"/>
+      <c r="G49" s="36"/>
+      <c r="H49" s="37"/>
     </row>
     <row r="50" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
@@ -1892,9 +2423,9 @@
       <c r="C50" s="4"/>
       <c r="D50" s="5"/>
       <c r="E50" s="23"/>
-      <c r="F50" s="34"/>
-      <c r="G50" s="35"/>
-      <c r="H50" s="36"/>
+      <c r="F50" s="35"/>
+      <c r="G50" s="36"/>
+      <c r="H50" s="37"/>
     </row>
     <row r="51" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
@@ -1902,9 +2433,9 @@
       <c r="C51" s="4"/>
       <c r="D51" s="5"/>
       <c r="E51" s="23"/>
-      <c r="F51" s="34"/>
-      <c r="G51" s="35"/>
-      <c r="H51" s="36"/>
+      <c r="F51" s="35"/>
+      <c r="G51" s="36"/>
+      <c r="H51" s="37"/>
     </row>
     <row r="52" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
@@ -1912,9 +2443,9 @@
       <c r="C52" s="4"/>
       <c r="D52" s="5"/>
       <c r="E52" s="23"/>
-      <c r="F52" s="34"/>
-      <c r="G52" s="35"/>
-      <c r="H52" s="36"/>
+      <c r="F52" s="35"/>
+      <c r="G52" s="36"/>
+      <c r="H52" s="37"/>
     </row>
     <row r="53" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3"/>
@@ -1922,9 +2453,9 @@
       <c r="C53" s="4"/>
       <c r="D53" s="5"/>
       <c r="E53" s="23"/>
-      <c r="F53" s="34"/>
-      <c r="G53" s="35"/>
-      <c r="H53" s="36"/>
+      <c r="F53" s="35"/>
+      <c r="G53" s="36"/>
+      <c r="H53" s="37"/>
     </row>
     <row r="54" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
@@ -1932,9 +2463,9 @@
       <c r="C54" s="4"/>
       <c r="D54" s="5"/>
       <c r="E54" s="23"/>
-      <c r="F54" s="34"/>
-      <c r="G54" s="35"/>
-      <c r="H54" s="36"/>
+      <c r="F54" s="35"/>
+      <c r="G54" s="36"/>
+      <c r="H54" s="37"/>
     </row>
     <row r="55" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3"/>
@@ -1942,9 +2473,9 @@
       <c r="C55" s="4"/>
       <c r="D55" s="5"/>
       <c r="E55" s="23"/>
-      <c r="F55" s="34"/>
-      <c r="G55" s="35"/>
-      <c r="H55" s="36"/>
+      <c r="F55" s="35"/>
+      <c r="G55" s="36"/>
+      <c r="H55" s="37"/>
     </row>
     <row r="56" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
@@ -1952,9 +2483,9 @@
       <c r="C56" s="4"/>
       <c r="D56" s="5"/>
       <c r="E56" s="23"/>
-      <c r="F56" s="34"/>
-      <c r="G56" s="35"/>
-      <c r="H56" s="36"/>
+      <c r="F56" s="35"/>
+      <c r="G56" s="36"/>
+      <c r="H56" s="37"/>
     </row>
     <row r="57" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
@@ -1962,9 +2493,9 @@
       <c r="C57" s="4"/>
       <c r="D57" s="5"/>
       <c r="E57" s="23"/>
-      <c r="F57" s="34"/>
-      <c r="G57" s="35"/>
-      <c r="H57" s="36"/>
+      <c r="F57" s="35"/>
+      <c r="G57" s="36"/>
+      <c r="H57" s="37"/>
     </row>
     <row r="58" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
@@ -1972,9 +2503,9 @@
       <c r="C58" s="4"/>
       <c r="D58" s="5"/>
       <c r="E58" s="23"/>
-      <c r="F58" s="34"/>
-      <c r="G58" s="35"/>
-      <c r="H58" s="36"/>
+      <c r="F58" s="35"/>
+      <c r="G58" s="36"/>
+      <c r="H58" s="37"/>
     </row>
     <row r="59" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3"/>
@@ -1982,9 +2513,9 @@
       <c r="C59" s="4"/>
       <c r="D59" s="5"/>
       <c r="E59" s="23"/>
-      <c r="F59" s="34"/>
-      <c r="G59" s="35"/>
-      <c r="H59" s="36"/>
+      <c r="F59" s="35"/>
+      <c r="G59" s="36"/>
+      <c r="H59" s="37"/>
     </row>
     <row r="60" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3"/>
@@ -1992,9 +2523,9 @@
       <c r="C60" s="4"/>
       <c r="D60" s="5"/>
       <c r="E60" s="23"/>
-      <c r="F60" s="34"/>
-      <c r="G60" s="35"/>
-      <c r="H60" s="36"/>
+      <c r="F60" s="35"/>
+      <c r="G60" s="36"/>
+      <c r="H60" s="37"/>
     </row>
     <row r="61" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3"/>
@@ -2002,9 +2533,9 @@
       <c r="C61" s="4"/>
       <c r="D61" s="5"/>
       <c r="E61" s="23"/>
-      <c r="F61" s="34"/>
-      <c r="G61" s="35"/>
-      <c r="H61" s="36"/>
+      <c r="F61" s="35"/>
+      <c r="G61" s="36"/>
+      <c r="H61" s="37"/>
     </row>
     <row r="62" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
@@ -2012,9 +2543,9 @@
       <c r="C62" s="4"/>
       <c r="D62" s="5"/>
       <c r="E62" s="23"/>
-      <c r="F62" s="34"/>
-      <c r="G62" s="35"/>
-      <c r="H62" s="36"/>
+      <c r="F62" s="35"/>
+      <c r="G62" s="36"/>
+      <c r="H62" s="37"/>
     </row>
     <row r="63" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3"/>
@@ -2022,9 +2553,9 @@
       <c r="C63" s="4"/>
       <c r="D63" s="5"/>
       <c r="E63" s="23"/>
-      <c r="F63" s="34"/>
-      <c r="G63" s="35"/>
-      <c r="H63" s="36"/>
+      <c r="F63" s="35"/>
+      <c r="G63" s="36"/>
+      <c r="H63" s="37"/>
     </row>
     <row r="64" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3"/>
@@ -2032,9 +2563,9 @@
       <c r="C64" s="4"/>
       <c r="D64" s="5"/>
       <c r="E64" s="23"/>
-      <c r="F64" s="34"/>
-      <c r="G64" s="35"/>
-      <c r="H64" s="36"/>
+      <c r="F64" s="35"/>
+      <c r="G64" s="36"/>
+      <c r="H64" s="37"/>
     </row>
     <row r="65" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3"/>
@@ -2042,9 +2573,9 @@
       <c r="C65" s="4"/>
       <c r="D65" s="5"/>
       <c r="E65" s="23"/>
-      <c r="F65" s="34"/>
-      <c r="G65" s="35"/>
-      <c r="H65" s="36"/>
+      <c r="F65" s="35"/>
+      <c r="G65" s="36"/>
+      <c r="H65" s="37"/>
     </row>
     <row r="66" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3"/>
@@ -2052,9 +2583,9 @@
       <c r="C66" s="4"/>
       <c r="D66" s="5"/>
       <c r="E66" s="23"/>
-      <c r="F66" s="34"/>
-      <c r="G66" s="35"/>
-      <c r="H66" s="36"/>
+      <c r="F66" s="35"/>
+      <c r="G66" s="36"/>
+      <c r="H66" s="37"/>
     </row>
     <row r="67" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
@@ -2062,9 +2593,9 @@
       <c r="C67" s="4"/>
       <c r="D67" s="5"/>
       <c r="E67" s="23"/>
-      <c r="F67" s="34"/>
-      <c r="G67" s="35"/>
-      <c r="H67" s="36"/>
+      <c r="F67" s="35"/>
+      <c r="G67" s="36"/>
+      <c r="H67" s="37"/>
     </row>
     <row r="68" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
@@ -2072,9 +2603,9 @@
       <c r="C68" s="4"/>
       <c r="D68" s="5"/>
       <c r="E68" s="23"/>
-      <c r="F68" s="34"/>
-      <c r="G68" s="35"/>
-      <c r="H68" s="36"/>
+      <c r="F68" s="35"/>
+      <c r="G68" s="36"/>
+      <c r="H68" s="37"/>
     </row>
     <row r="69" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3"/>
@@ -2082,9 +2613,9 @@
       <c r="C69" s="4"/>
       <c r="D69" s="5"/>
       <c r="E69" s="23"/>
-      <c r="F69" s="34"/>
-      <c r="G69" s="35"/>
-      <c r="H69" s="36"/>
+      <c r="F69" s="35"/>
+      <c r="G69" s="36"/>
+      <c r="H69" s="37"/>
     </row>
     <row r="70" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3"/>
@@ -2092,9 +2623,9 @@
       <c r="C70" s="4"/>
       <c r="D70" s="5"/>
       <c r="E70" s="23"/>
-      <c r="F70" s="34"/>
-      <c r="G70" s="35"/>
-      <c r="H70" s="36"/>
+      <c r="F70" s="35"/>
+      <c r="G70" s="36"/>
+      <c r="H70" s="37"/>
     </row>
     <row r="71" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="3"/>
@@ -2102,9 +2633,9 @@
       <c r="C71" s="4"/>
       <c r="D71" s="5"/>
       <c r="E71" s="23"/>
-      <c r="F71" s="34"/>
-      <c r="G71" s="35"/>
-      <c r="H71" s="36"/>
+      <c r="F71" s="35"/>
+      <c r="G71" s="36"/>
+      <c r="H71" s="37"/>
     </row>
     <row r="72" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
@@ -2112,9 +2643,9 @@
       <c r="C72" s="4"/>
       <c r="D72" s="5"/>
       <c r="E72" s="23"/>
-      <c r="F72" s="34"/>
-      <c r="G72" s="35"/>
-      <c r="H72" s="36"/>
+      <c r="F72" s="35"/>
+      <c r="G72" s="36"/>
+      <c r="H72" s="37"/>
     </row>
     <row r="73" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="3"/>
@@ -2122,9 +2653,9 @@
       <c r="C73" s="4"/>
       <c r="D73" s="5"/>
       <c r="E73" s="23"/>
-      <c r="F73" s="34"/>
-      <c r="G73" s="35"/>
-      <c r="H73" s="36"/>
+      <c r="F73" s="35"/>
+      <c r="G73" s="36"/>
+      <c r="H73" s="37"/>
     </row>
     <row r="74" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
@@ -2132,9 +2663,9 @@
       <c r="C74" s="4"/>
       <c r="D74" s="5"/>
       <c r="E74" s="23"/>
-      <c r="F74" s="34"/>
-      <c r="G74" s="35"/>
-      <c r="H74" s="36"/>
+      <c r="F74" s="35"/>
+      <c r="G74" s="36"/>
+      <c r="H74" s="37"/>
     </row>
     <row r="75" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="3"/>
@@ -2142,9 +2673,9 @@
       <c r="C75" s="4"/>
       <c r="D75" s="5"/>
       <c r="E75" s="23"/>
-      <c r="F75" s="34"/>
-      <c r="G75" s="35"/>
-      <c r="H75" s="36"/>
+      <c r="F75" s="35"/>
+      <c r="G75" s="36"/>
+      <c r="H75" s="37"/>
     </row>
     <row r="76" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
@@ -2152,9 +2683,9 @@
       <c r="C76" s="4"/>
       <c r="D76" s="5"/>
       <c r="E76" s="23"/>
-      <c r="F76" s="34"/>
-      <c r="G76" s="35"/>
-      <c r="H76" s="36"/>
+      <c r="F76" s="35"/>
+      <c r="G76" s="36"/>
+      <c r="H76" s="37"/>
     </row>
     <row r="77" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="3"/>
@@ -2162,9 +2693,9 @@
       <c r="C77" s="4"/>
       <c r="D77" s="5"/>
       <c r="E77" s="23"/>
-      <c r="F77" s="34"/>
-      <c r="G77" s="35"/>
-      <c r="H77" s="36"/>
+      <c r="F77" s="35"/>
+      <c r="G77" s="36"/>
+      <c r="H77" s="37"/>
     </row>
     <row r="78" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="3"/>
@@ -2172,9 +2703,9 @@
       <c r="C78" s="4"/>
       <c r="D78" s="5"/>
       <c r="E78" s="23"/>
-      <c r="F78" s="34"/>
-      <c r="G78" s="35"/>
-      <c r="H78" s="36"/>
+      <c r="F78" s="35"/>
+      <c r="G78" s="36"/>
+      <c r="H78" s="37"/>
     </row>
     <row r="79" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="3"/>
@@ -2182,9 +2713,9 @@
       <c r="C79" s="4"/>
       <c r="D79" s="5"/>
       <c r="E79" s="23"/>
-      <c r="F79" s="34"/>
-      <c r="G79" s="35"/>
-      <c r="H79" s="36"/>
+      <c r="F79" s="35"/>
+      <c r="G79" s="36"/>
+      <c r="H79" s="37"/>
     </row>
     <row r="80" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="3"/>
@@ -2192,9 +2723,9 @@
       <c r="C80" s="4"/>
       <c r="D80" s="5"/>
       <c r="E80" s="23"/>
-      <c r="F80" s="34"/>
-      <c r="G80" s="35"/>
-      <c r="H80" s="36"/>
+      <c r="F80" s="35"/>
+      <c r="G80" s="36"/>
+      <c r="H80" s="37"/>
     </row>
     <row r="81" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="3"/>
@@ -2202,9 +2733,9 @@
       <c r="C81" s="4"/>
       <c r="D81" s="5"/>
       <c r="E81" s="23"/>
-      <c r="F81" s="34"/>
-      <c r="G81" s="35"/>
-      <c r="H81" s="36"/>
+      <c r="F81" s="35"/>
+      <c r="G81" s="36"/>
+      <c r="H81" s="37"/>
     </row>
     <row r="82" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="3"/>
@@ -2212,9 +2743,9 @@
       <c r="C82" s="4"/>
       <c r="D82" s="5"/>
       <c r="E82" s="23"/>
-      <c r="F82" s="34"/>
-      <c r="G82" s="35"/>
-      <c r="H82" s="36"/>
+      <c r="F82" s="35"/>
+      <c r="G82" s="36"/>
+      <c r="H82" s="37"/>
     </row>
     <row r="83" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="3"/>
@@ -2222,9 +2753,9 @@
       <c r="C83" s="4"/>
       <c r="D83" s="5"/>
       <c r="E83" s="23"/>
-      <c r="F83" s="34"/>
-      <c r="G83" s="35"/>
-      <c r="H83" s="36"/>
+      <c r="F83" s="35"/>
+      <c r="G83" s="36"/>
+      <c r="H83" s="37"/>
     </row>
     <row r="84" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="3"/>
@@ -2232,9 +2763,9 @@
       <c r="C84" s="4"/>
       <c r="D84" s="5"/>
       <c r="E84" s="23"/>
-      <c r="F84" s="34"/>
-      <c r="G84" s="35"/>
-      <c r="H84" s="36"/>
+      <c r="F84" s="35"/>
+      <c r="G84" s="36"/>
+      <c r="H84" s="37"/>
     </row>
     <row r="85" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="3"/>
@@ -2242,9 +2773,9 @@
       <c r="C85" s="4"/>
       <c r="D85" s="5"/>
       <c r="E85" s="23"/>
-      <c r="F85" s="34"/>
-      <c r="G85" s="35"/>
-      <c r="H85" s="36"/>
+      <c r="F85" s="35"/>
+      <c r="G85" s="36"/>
+      <c r="H85" s="37"/>
     </row>
     <row r="86" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="3"/>
@@ -2252,9 +2783,9 @@
       <c r="C86" s="4"/>
       <c r="D86" s="5"/>
       <c r="E86" s="23"/>
-      <c r="F86" s="34"/>
-      <c r="G86" s="35"/>
-      <c r="H86" s="36"/>
+      <c r="F86" s="35"/>
+      <c r="G86" s="36"/>
+      <c r="H86" s="37"/>
     </row>
     <row r="87" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="3"/>
@@ -2262,9 +2793,9 @@
       <c r="C87" s="4"/>
       <c r="D87" s="5"/>
       <c r="E87" s="23"/>
-      <c r="F87" s="34"/>
-      <c r="G87" s="35"/>
-      <c r="H87" s="36"/>
+      <c r="F87" s="35"/>
+      <c r="G87" s="36"/>
+      <c r="H87" s="37"/>
     </row>
     <row r="88" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="3"/>
@@ -2272,9 +2803,9 @@
       <c r="C88" s="4"/>
       <c r="D88" s="5"/>
       <c r="E88" s="23"/>
-      <c r="F88" s="34"/>
-      <c r="G88" s="35"/>
-      <c r="H88" s="36"/>
+      <c r="F88" s="35"/>
+      <c r="G88" s="36"/>
+      <c r="H88" s="37"/>
     </row>
     <row r="89" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="3"/>
@@ -2282,9 +2813,9 @@
       <c r="C89" s="4"/>
       <c r="D89" s="5"/>
       <c r="E89" s="23"/>
-      <c r="F89" s="34"/>
-      <c r="G89" s="35"/>
-      <c r="H89" s="36"/>
+      <c r="F89" s="35"/>
+      <c r="G89" s="36"/>
+      <c r="H89" s="37"/>
     </row>
     <row r="90" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="3"/>
@@ -2292,9 +2823,9 @@
       <c r="C90" s="4"/>
       <c r="D90" s="5"/>
       <c r="E90" s="23"/>
-      <c r="F90" s="34"/>
-      <c r="G90" s="35"/>
-      <c r="H90" s="36"/>
+      <c r="F90" s="35"/>
+      <c r="G90" s="36"/>
+      <c r="H90" s="37"/>
     </row>
     <row r="91" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="3"/>
@@ -2302,9 +2833,9 @@
       <c r="C91" s="4"/>
       <c r="D91" s="5"/>
       <c r="E91" s="23"/>
-      <c r="F91" s="34"/>
-      <c r="G91" s="35"/>
-      <c r="H91" s="36"/>
+      <c r="F91" s="35"/>
+      <c r="G91" s="36"/>
+      <c r="H91" s="37"/>
     </row>
     <row r="92" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="3"/>
@@ -2312,9 +2843,9 @@
       <c r="C92" s="4"/>
       <c r="D92" s="5"/>
       <c r="E92" s="23"/>
-      <c r="F92" s="34"/>
-      <c r="G92" s="35"/>
-      <c r="H92" s="36"/>
+      <c r="F92" s="35"/>
+      <c r="G92" s="36"/>
+      <c r="H92" s="37"/>
     </row>
     <row r="93" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="3"/>
@@ -2322,9 +2853,9 @@
       <c r="C93" s="4"/>
       <c r="D93" s="5"/>
       <c r="E93" s="23"/>
-      <c r="F93" s="34"/>
-      <c r="G93" s="35"/>
-      <c r="H93" s="36"/>
+      <c r="F93" s="35"/>
+      <c r="G93" s="36"/>
+      <c r="H93" s="37"/>
     </row>
     <row r="94" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="3"/>
@@ -2332,9 +2863,9 @@
       <c r="C94" s="4"/>
       <c r="D94" s="5"/>
       <c r="E94" s="23"/>
-      <c r="F94" s="34"/>
-      <c r="G94" s="35"/>
-      <c r="H94" s="36"/>
+      <c r="F94" s="35"/>
+      <c r="G94" s="36"/>
+      <c r="H94" s="37"/>
     </row>
     <row r="95" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="3"/>
@@ -2342,9 +2873,9 @@
       <c r="C95" s="4"/>
       <c r="D95" s="5"/>
       <c r="E95" s="23"/>
-      <c r="F95" s="34"/>
-      <c r="G95" s="35"/>
-      <c r="H95" s="36"/>
+      <c r="F95" s="35"/>
+      <c r="G95" s="36"/>
+      <c r="H95" s="37"/>
     </row>
     <row r="96" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="3"/>
@@ -2352,9 +2883,9 @@
       <c r="C96" s="4"/>
       <c r="D96" s="5"/>
       <c r="E96" s="23"/>
-      <c r="F96" s="34"/>
-      <c r="G96" s="35"/>
-      <c r="H96" s="36"/>
+      <c r="F96" s="35"/>
+      <c r="G96" s="36"/>
+      <c r="H96" s="37"/>
     </row>
     <row r="97" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="3"/>
@@ -2362,9 +2893,9 @@
       <c r="C97" s="4"/>
       <c r="D97" s="5"/>
       <c r="E97" s="23"/>
-      <c r="F97" s="34"/>
-      <c r="G97" s="35"/>
-      <c r="H97" s="36"/>
+      <c r="F97" s="35"/>
+      <c r="G97" s="36"/>
+      <c r="H97" s="37"/>
     </row>
     <row r="98" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3"/>
@@ -2372,9 +2903,9 @@
       <c r="C98" s="4"/>
       <c r="D98" s="5"/>
       <c r="E98" s="23"/>
-      <c r="F98" s="34"/>
-      <c r="G98" s="35"/>
-      <c r="H98" s="36"/>
+      <c r="F98" s="35"/>
+      <c r="G98" s="36"/>
+      <c r="H98" s="37"/>
     </row>
     <row r="99" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="3"/>
@@ -2382,9 +2913,9 @@
       <c r="C99" s="4"/>
       <c r="D99" s="5"/>
       <c r="E99" s="23"/>
-      <c r="F99" s="34"/>
-      <c r="G99" s="35"/>
-      <c r="H99" s="36"/>
+      <c r="F99" s="35"/>
+      <c r="G99" s="36"/>
+      <c r="H99" s="37"/>
     </row>
     <row r="100" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="3"/>
@@ -2392,9 +2923,9 @@
       <c r="C100" s="4"/>
       <c r="D100" s="5"/>
       <c r="E100" s="23"/>
-      <c r="F100" s="34"/>
-      <c r="G100" s="35"/>
-      <c r="H100" s="36"/>
+      <c r="F100" s="35"/>
+      <c r="G100" s="36"/>
+      <c r="H100" s="37"/>
     </row>
     <row r="101" spans="1:8" ht="39" hidden="1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -2535,77 +3066,77 @@
       <c r="A1" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="58"/>
     </row>
     <row r="2" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="60"/>
     </row>
     <row r="3" spans="1:5" ht="135.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="60"/>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="61"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="62"/>
     </row>
     <row r="4" spans="1:5" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="64"/>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="66"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="66"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="67"/>
     </row>
     <row r="5" spans="1:5" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="60"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="61"/>
+      <c r="B5" s="61"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="62"/>
     </row>
     <row r="6" spans="1:5" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="60"/>
-      <c r="C6" s="60"/>
-      <c r="D6" s="60"/>
-      <c r="E6" s="61"/>
+      <c r="B6" s="61"/>
+      <c r="C6" s="61"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="62"/>
     </row>
     <row r="7" spans="1:5" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="64"/>
-      <c r="C7" s="65"/>
-      <c r="D7" s="65"/>
-      <c r="E7" s="66"/>
+      <c r="B7" s="65"/>
+      <c r="C7" s="66"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="67"/>
     </row>
     <row r="8" spans="1:5" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="62"/>
-      <c r="C8" s="62"/>
-      <c r="D8" s="62"/>
-      <c r="E8" s="63"/>
+      <c r="B8" s="63"/>
+      <c r="C8" s="63"/>
+      <c r="D8" s="63"/>
+      <c r="E8" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -2633,7 +3164,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B4" sqref="B4:G4"/>
     </sheetView>
   </sheetViews>
@@ -2646,178 +3177,178 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="69"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="70"/>
     </row>
     <row r="2" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="78">
+      <c r="B2" s="79">
         <v>41722</v>
       </c>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="62"/>
     </row>
     <row r="3" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="60" t="s">
+      <c r="B3" s="61" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="61"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="62"/>
     </row>
     <row r="4" spans="1:7" ht="111.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="61" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="61"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="62"/>
     </row>
     <row r="5" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="62"/>
-      <c r="C5" s="62"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="63"/>
+      <c r="B5" s="63"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="64"/>
     </row>
     <row r="6" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="67" t="s">
+      <c r="A7" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="68"/>
-      <c r="C7" s="68"/>
-      <c r="D7" s="68"/>
-      <c r="E7" s="68"/>
-      <c r="F7" s="68"/>
-      <c r="G7" s="69"/>
+      <c r="B7" s="69"/>
+      <c r="C7" s="69"/>
+      <c r="D7" s="69"/>
+      <c r="E7" s="69"/>
+      <c r="F7" s="69"/>
+      <c r="G7" s="70"/>
     </row>
     <row r="8" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="74"/>
-      <c r="C8" s="74"/>
-      <c r="D8" s="74"/>
-      <c r="E8" s="74"/>
-      <c r="F8" s="74"/>
-      <c r="G8" s="75"/>
+      <c r="B8" s="75"/>
+      <c r="C8" s="75"/>
+      <c r="D8" s="75"/>
+      <c r="E8" s="75"/>
+      <c r="F8" s="75"/>
+      <c r="G8" s="76"/>
     </row>
     <row r="9" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="60"/>
-      <c r="C9" s="60"/>
-      <c r="D9" s="60"/>
-      <c r="E9" s="60"/>
-      <c r="F9" s="60"/>
-      <c r="G9" s="61"/>
+      <c r="B9" s="61"/>
+      <c r="C9" s="61"/>
+      <c r="D9" s="61"/>
+      <c r="E9" s="61"/>
+      <c r="F9" s="61"/>
+      <c r="G9" s="62"/>
     </row>
     <row r="10" spans="1:7" ht="111.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="60"/>
-      <c r="C10" s="60"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="60"/>
-      <c r="F10" s="60"/>
-      <c r="G10" s="61"/>
+      <c r="B10" s="61"/>
+      <c r="C10" s="61"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="61"/>
+      <c r="G10" s="62"/>
     </row>
     <row r="11" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="76"/>
-      <c r="C11" s="76"/>
-      <c r="D11" s="76"/>
-      <c r="E11" s="76"/>
-      <c r="F11" s="76"/>
-      <c r="G11" s="77"/>
+      <c r="B11" s="77"/>
+      <c r="C11" s="77"/>
+      <c r="D11" s="77"/>
+      <c r="E11" s="77"/>
+      <c r="F11" s="77"/>
+      <c r="G11" s="78"/>
     </row>
     <row r="12" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="67" t="s">
+      <c r="A14" s="68" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="68"/>
-      <c r="C14" s="68"/>
-      <c r="D14" s="68"/>
-      <c r="E14" s="68"/>
-      <c r="F14" s="68"/>
-      <c r="G14" s="69"/>
+      <c r="B14" s="69"/>
+      <c r="C14" s="69"/>
+      <c r="D14" s="69"/>
+      <c r="E14" s="69"/>
+      <c r="F14" s="69"/>
+      <c r="G14" s="70"/>
     </row>
     <row r="15" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="70"/>
-      <c r="C15" s="70"/>
-      <c r="D15" s="70"/>
-      <c r="E15" s="70"/>
-      <c r="F15" s="70"/>
-      <c r="G15" s="71"/>
+      <c r="B15" s="71"/>
+      <c r="C15" s="71"/>
+      <c r="D15" s="71"/>
+      <c r="E15" s="71"/>
+      <c r="F15" s="71"/>
+      <c r="G15" s="72"/>
     </row>
     <row r="16" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="60"/>
-      <c r="C16" s="60"/>
-      <c r="D16" s="60"/>
-      <c r="E16" s="60"/>
-      <c r="F16" s="60"/>
-      <c r="G16" s="61"/>
+      <c r="B16" s="61"/>
+      <c r="C16" s="61"/>
+      <c r="D16" s="61"/>
+      <c r="E16" s="61"/>
+      <c r="F16" s="61"/>
+      <c r="G16" s="62"/>
     </row>
     <row r="17" spans="1:7" ht="113.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="60"/>
-      <c r="C17" s="60"/>
-      <c r="D17" s="60"/>
-      <c r="E17" s="60"/>
-      <c r="F17" s="60"/>
-      <c r="G17" s="61"/>
+      <c r="B17" s="61"/>
+      <c r="C17" s="61"/>
+      <c r="D17" s="61"/>
+      <c r="E17" s="61"/>
+      <c r="F17" s="61"/>
+      <c r="G17" s="62"/>
     </row>
     <row r="18" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="72"/>
-      <c r="C18" s="72"/>
-      <c r="D18" s="72"/>
-      <c r="E18" s="72"/>
-      <c r="F18" s="72"/>
-      <c r="G18" s="73"/>
+      <c r="B18" s="73"/>
+      <c r="C18" s="73"/>
+      <c r="D18" s="73"/>
+      <c r="E18" s="73"/>
+      <c r="F18" s="73"/>
+      <c r="G18" s="74"/>
     </row>
     <row r="19" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:7" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>